<commit_message>
Update email settings and logger in IMAPFlow constructor, delete backup.json
</commit_message>
<xml_diff>
--- a/data/تجربة ايميلات موبايلي.xlsx
+++ b/data/تجربة ايميلات موبايلي.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t xml:space="preserve">رقم الخدمة</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">R@hotmail.it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01/28/ 2021</t>
   </si>
 </sst>
 </file>
@@ -334,10 +331,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.71"/>
@@ -432,9 +429,7 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" s="0"/>
       <c r="F4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>